<commit_message>
sum payments by accounts
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lori/Desktop/Repos/payg-solar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458193F-EE49-5245-A805-E34691815A0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A399D4D-3AC2-954C-B78E-5F29992669BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17460" yWindow="6260" windowWidth="16080" windowHeight="8460" xr2:uid="{241756B6-0FD0-1949-A44E-56B401490B1B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>account_state_transition</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>type</t>
+  </si>
+  <si>
+    <t>(14762, 7)</t>
+  </si>
+  <si>
+    <t>(772, 6)</t>
+  </si>
+  <si>
+    <t>(107, 3)</t>
+  </si>
+  <si>
+    <t>(42, 6)</t>
+  </si>
+  <si>
+    <t>(9452, 5)</t>
+  </si>
+  <si>
+    <t>(42, 3)</t>
   </si>
 </sst>
 </file>
@@ -461,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D25B8779-D69B-9142-804F-1BC39AADA0B5}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -477,133 +495,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>